<commit_message>
V 3.8.8 CCB perfeccionado y mejorada la sincronización de ítems
</commit_message>
<xml_diff>
--- a/CONTROL DE BUFFERS/PLANTILLAS/Plantilla Copiado Pegado.xlsx
+++ b/CONTROL DE BUFFERS/PLANTILLAS/Plantilla Copiado Pegado.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TEXTO ORIGINAL</t>
   </si>
@@ -38,23 +38,26 @@
     <t>NÚMERO PARA RAMCAS</t>
   </si>
   <si>
-    <t>12122</t>
-  </si>
-  <si>
     <t>¿ES TEXTO?</t>
   </si>
   <si>
     <t>¿ES NÚMERO?</t>
   </si>
   <si>
-    <t>Plantilla de Copiado y Pegado</t>
+    <t>Plantilla de Copiado y Pegado de RAMCAS</t>
+  </si>
+  <si>
+    <t>PARA INGRESAR TEXTOS A RAMCAS</t>
+  </si>
+  <si>
+    <t>PARA INGRESAR NÚMEROS A RAMCAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,8 +72,16 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,8 +100,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -98,12 +121,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,10 +193,29 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título" xfId="1" builtinId="15"/>
+    <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -163,13 +254,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>847724</xdr:rowOff>
+      <xdr:rowOff>361951</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -178,8 +269,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="28575" y="323850"/>
-          <a:ext cx="7324725" cy="819149"/>
+          <a:off x="28575" y="390526"/>
+          <a:ext cx="7410450" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -218,13 +309,94 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-EC" sz="1100"/>
-            <a:t>Antes</a:t>
+            <a:t>Antes de copiar cualquier valor a RAMCAS es necesario depurarlo:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>419101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28575" y="714376"/>
+          <a:ext cx="7410450" cy="695324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>¿El valor que se va a pegar en RAMCAS es un Texto?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>Pegar</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-EC" sz="1100" baseline="0"/>
-            <a:t> de copiar los datos a RAMCAS, hay que depurarlos. Se tienen que pegar los valores originales en las columnas TEXTO ORIGINAL y/o NÚMERO ORIGINAL, donde corresponda según su naturaleza. Excel convertirá esos datos para que sean aptos para pegarlos en RAMCAS, y éstos están en las columnas TEXTO PARA RAMCAS y NÚMERO PARA RAMCAS. No reemplazar las fórmulas. Sólo Eliminar Filas de Tabla cuando se necesite copiar y pegar nuevos datos.</a:t>
+            <a:rPr lang="es-EC" baseline="0">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> los valores originales en la columna TEXTO ORIGINAL. Copiar los las celdas de la columna TEXTO PARA RAMCAS y pegarla dentro de RAMCAS con Pegar Valores. Hacer lo correspondiente con datos numéricos, pero en los campos de NÚMERO.</a:t>
           </a:r>
-          <a:endParaRPr lang="es-EC" sz="1100"/>
+          <a:endParaRPr lang="es-EC">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -234,22 +406,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Conversion" displayName="Conversion" ref="A3:F4" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A3:F4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Conversion" displayName="Conversion" ref="A5:F6" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A5:F6"/>
   <tableColumns count="6">
     <tableColumn id="1" name="TEXTO ORIGINAL" dataDxfId="3"/>
     <tableColumn id="2" name="TEXTO PARA RAMCAS">
       <calculatedColumnFormula>CLEAN(TRIM(Conversion[TEXTO ORIGINAL]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="¿ES TEXTO?" dataDxfId="2">
-      <calculatedColumnFormula>--ISTEXT(Conversion[TEXTO PARA RAMCAS])</calculatedColumnFormula>
+      <calculatedColumnFormula>ISTEXT(Conversion[[#This Row],[TEXTO PARA RAMCAS]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="NÚMERO ORIGINAL" dataDxfId="1"/>
     <tableColumn id="4" name="NÚMERO PARA RAMCAS">
-      <calculatedColumnFormula>Conversion[NÚMERO ORIGINAL]*1</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(Conversion[NÚMERO ORIGINAL]*1,"Ingresar número")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="¿ES NÚMERO?" dataDxfId="0">
-      <calculatedColumnFormula>--ISNUMBER(Conversion[NÚMERO PARA RAMCAS])</calculatedColumnFormula>
+      <calculatedColumnFormula>ISNUMBER(Conversion[[#This Row],[NÚMERO PARA RAMCAS]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -519,13 +691,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
@@ -533,51 +708,64 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
     </row>
-    <row r="2" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>12345</v>
+      </c>
+      <c r="B6" t="str">
+        <f>CLEAN(TRIM(Conversion[TEXTO ORIGINAL]))</f>
+        <v>12345</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <f>ISTEXT(Conversion[[#This Row],[TEXTO PARA RAMCAS]])</f>
         <v>1</v>
       </c>
-      <c r="B4" t="str">
-        <f>CLEAN(TRIM(Conversion[TEXTO ORIGINAL]))</f>
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <f>--ISTEXT(Conversion[TEXTO PARA RAMCAS])</f>
+      <c r="E6">
+        <f>IFERROR(Conversion[NÚMERO ORIGINAL]*1,"Ingresar número")</f>
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <f>Conversion[NÚMERO ORIGINAL]*1</f>
-        <v>12122</v>
-      </c>
-      <c r="F4" s="1">
-        <f>--ISNUMBER(Conversion[NÚMERO PARA RAMCAS])</f>
+      <c r="F6" s="1" t="b">
+        <f>ISNUMBER(Conversion[[#This Row],[NÚMERO PARA RAMCAS]])</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>